<commit_message>
test switch languages done
</commit_message>
<xml_diff>
--- a/com.bankofamerica/src/test/resources/test_data.xlsx
+++ b/com.bankofamerica/src/test/resources/test_data.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sadou\IdeaProjects\SeleniumBootcamp\com.bankofamerica\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B694381B-F845-48A9-B10C-4902B3157289}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A462DF1C-7FBC-46AC-81E1-95D728708762}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{2B44F5B2-02D3-40B2-8D0E-7869D45C0BD3}"/>
+    <workbookView xWindow="1260" yWindow="984" windowWidth="17280" windowHeight="8880" activeTab="1" xr2:uid="{2B44F5B2-02D3-40B2-8D0E-7869D45C0BD3}"/>
   </bookViews>
   <sheets>
     <sheet name="doSearchAtmLocation" sheetId="1" r:id="rId1"/>
+    <sheet name="invalidZip" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,9 +35,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
     <t>zipCode</t>
+  </si>
+  <si>
+    <t>invalidZip</t>
   </si>
 </sst>
 </file>
@@ -390,7 +394,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D821A093-4A5C-47F9-BCC6-9599719CA6A3}">
   <dimension ref="A1:A4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
@@ -419,4 +423,39 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D50139F-5A0B-4764-891A-17ABEDD14782}">
+  <dimension ref="A1:A4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>789</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>